<commit_message>
Added error pages, 1st draft of overview
</commit_message>
<xml_diff>
--- a/dash_app/data/data_for_main_table.xlsx
+++ b/dash_app/data/data_for_main_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\citco\Documents\Projects\Platt&amp;Reilly\Projects\dashboard\src\assets\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\citco\Documents\Projects\Platt&amp;Reilly\Projects\dashboard\dash_app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5491BA48-19F6-4CBC-A191-B24BB06F1F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DCE9E9A-DFA5-47E9-94CE-8A6CBB7B2B42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24750" yWindow="2985" windowWidth="21600" windowHeight="11385" xr2:uid="{7D4D2C26-5603-43D3-8ABB-FFEB205B5079}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7D4D2C26-5603-43D3-8ABB-FFEB205B5079}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>Project Name</t>
   </si>
@@ -92,97 +92,7 @@
     <t>KINGS KROSS</t>
   </si>
   <si>
-    <t>Apr 23 - Apr 24 (53)</t>
-  </si>
-  <si>
-    <t>2 430 K</t>
-  </si>
-  <si>
-    <t>12 430 K</t>
-  </si>
-  <si>
-    <t>8 500 K</t>
-  </si>
-  <si>
-    <t>2 850 K</t>
-  </si>
-  <si>
-    <t>8 850 K</t>
-  </si>
-  <si>
-    <t>6 800 K</t>
-  </si>
-  <si>
-    <t>570 K</t>
-  </si>
-  <si>
-    <t>1 570 K</t>
-  </si>
-  <si>
-    <t>1 205 K</t>
-  </si>
-  <si>
-    <t>280 K</t>
-  </si>
-  <si>
-    <t>1 400 K</t>
-  </si>
-  <si>
-    <t>985 K</t>
-  </si>
-  <si>
-    <t>530 K</t>
-  </si>
-  <si>
-    <t>1 380 K</t>
-  </si>
-  <si>
-    <t>1 100 K</t>
-  </si>
-  <si>
-    <t>250 K</t>
-  </si>
-  <si>
-    <t>1 250 K</t>
-  </si>
-  <si>
-    <t>900 K</t>
-  </si>
-  <si>
-    <t>550 K</t>
-  </si>
-  <si>
-    <t>1 420 K</t>
-  </si>
-  <si>
-    <t>1 050 K</t>
-  </si>
-  <si>
-    <t>245 K</t>
-  </si>
-  <si>
-    <t>1 234 K</t>
-  </si>
-  <si>
-    <t>905 K</t>
-  </si>
-  <si>
-    <t>2 000 K</t>
-  </si>
-  <si>
-    <t>6 000 K</t>
-  </si>
-  <si>
-    <t>3 000 K</t>
-  </si>
-  <si>
-    <t>4 000 K</t>
-  </si>
-  <si>
-    <t>5 000 K</t>
-  </si>
-  <si>
-    <t>7 000 K</t>
+    <t>Apr 23-Apr 24 (53)</t>
   </si>
 </sst>
 </file>
@@ -569,7 +479,7 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,29 +539,29 @@
       <c r="C2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I2" t="s">
-        <v>43</v>
-      </c>
-      <c r="J2" t="s">
-        <v>43</v>
-      </c>
-      <c r="K2" t="s">
-        <v>43</v>
+      <c r="D2">
+        <v>2430</v>
+      </c>
+      <c r="E2">
+        <v>570</v>
+      </c>
+      <c r="F2">
+        <v>530</v>
+      </c>
+      <c r="G2">
+        <v>550</v>
+      </c>
+      <c r="H2">
+        <v>2000</v>
+      </c>
+      <c r="I2">
+        <v>2000</v>
+      </c>
+      <c r="J2">
+        <v>2000</v>
+      </c>
+      <c r="K2">
+        <v>2000</v>
       </c>
       <c r="L2">
         <v>19</v>
@@ -667,29 +577,29 @@
       <c r="C3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J3" t="s">
-        <v>45</v>
-      </c>
-      <c r="K3" t="s">
-        <v>45</v>
+      <c r="D3">
+        <v>12430</v>
+      </c>
+      <c r="E3">
+        <v>1570</v>
+      </c>
+      <c r="F3">
+        <v>1380</v>
+      </c>
+      <c r="G3">
+        <v>1420</v>
+      </c>
+      <c r="H3">
+        <v>3000</v>
+      </c>
+      <c r="I3">
+        <v>3000</v>
+      </c>
+      <c r="J3">
+        <v>3000</v>
+      </c>
+      <c r="K3">
+        <v>3000</v>
       </c>
       <c r="L3">
         <v>20</v>
@@ -705,29 +615,29 @@
       <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" t="s">
-        <v>46</v>
-      </c>
-      <c r="I4" t="s">
-        <v>46</v>
-      </c>
-      <c r="J4" t="s">
-        <v>46</v>
-      </c>
-      <c r="K4" t="s">
-        <v>46</v>
+      <c r="D4">
+        <v>8500</v>
+      </c>
+      <c r="E4">
+        <v>1205</v>
+      </c>
+      <c r="F4">
+        <v>1100</v>
+      </c>
+      <c r="G4">
+        <v>1050</v>
+      </c>
+      <c r="H4">
+        <v>4000</v>
+      </c>
+      <c r="I4">
+        <v>4000</v>
+      </c>
+      <c r="J4">
+        <v>4000</v>
+      </c>
+      <c r="K4">
+        <v>4000</v>
       </c>
       <c r="L4">
         <v>21</v>
@@ -743,29 +653,29 @@
       <c r="C5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" t="s">
-        <v>40</v>
-      </c>
-      <c r="H5" t="s">
-        <v>47</v>
-      </c>
-      <c r="I5" t="s">
-        <v>47</v>
-      </c>
-      <c r="J5" t="s">
-        <v>47</v>
-      </c>
-      <c r="K5" t="s">
-        <v>47</v>
+      <c r="D5">
+        <v>2850</v>
+      </c>
+      <c r="E5">
+        <v>280</v>
+      </c>
+      <c r="F5">
+        <v>250</v>
+      </c>
+      <c r="G5">
+        <v>245</v>
+      </c>
+      <c r="H5">
+        <v>5000</v>
+      </c>
+      <c r="I5">
+        <v>5000</v>
+      </c>
+      <c r="J5">
+        <v>5000</v>
+      </c>
+      <c r="K5">
+        <v>5000</v>
       </c>
       <c r="L5">
         <v>22</v>
@@ -781,29 +691,29 @@
       <c r="C6" t="s">
         <v>18</v>
       </c>
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H6" t="s">
-        <v>44</v>
-      </c>
-      <c r="I6" t="s">
-        <v>44</v>
-      </c>
-      <c r="J6" t="s">
-        <v>44</v>
-      </c>
-      <c r="K6" t="s">
-        <v>44</v>
+      <c r="D6">
+        <v>8850</v>
+      </c>
+      <c r="E6">
+        <v>1400</v>
+      </c>
+      <c r="F6">
+        <v>1250</v>
+      </c>
+      <c r="G6">
+        <v>1234</v>
+      </c>
+      <c r="H6">
+        <v>6000</v>
+      </c>
+      <c r="I6">
+        <v>6000</v>
+      </c>
+      <c r="J6">
+        <v>6000</v>
+      </c>
+      <c r="K6">
+        <v>6000</v>
       </c>
       <c r="L6">
         <v>23</v>
@@ -819,29 +729,29 @@
       <c r="C7" t="s">
         <v>18</v>
       </c>
-      <c r="D7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" t="s">
-        <v>42</v>
-      </c>
-      <c r="H7" t="s">
-        <v>48</v>
-      </c>
-      <c r="I7" t="s">
-        <v>48</v>
-      </c>
-      <c r="J7" t="s">
-        <v>48</v>
-      </c>
-      <c r="K7" t="s">
-        <v>48</v>
+      <c r="D7">
+        <v>6800</v>
+      </c>
+      <c r="E7">
+        <v>985</v>
+      </c>
+      <c r="F7">
+        <v>900</v>
+      </c>
+      <c r="G7">
+        <v>905</v>
+      </c>
+      <c r="H7">
+        <v>7000</v>
+      </c>
+      <c r="I7">
+        <v>7000</v>
+      </c>
+      <c r="J7">
+        <v>7000</v>
+      </c>
+      <c r="K7">
+        <v>7000</v>
       </c>
       <c r="L7">
         <v>24</v>

</xml_diff>

<commit_message>
Integrated collapses, maps, changing charts based on project selection
</commit_message>
<xml_diff>
--- a/dash_app/data/data_for_main_table.xlsx
+++ b/dash_app/data/data_for_main_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\citco\Documents\Projects\Platt&amp;Reilly\Projects\dashboard\dash_app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1073218D-55CB-4FC5-8730-EA37C1B90859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6ABE197-23B7-46FB-84F8-478921827F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7D4D2C26-5603-43D3-8ABB-FFEB205B5079}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7D4D2C26-5603-43D3-8ABB-FFEB205B5079}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -549,7 +549,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7:XFD7"/>
+      <selection pane="bottomLeft" activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2196,7 +2196,7 @@
         <v>7000</v>
       </c>
       <c r="L40" s="16">
-        <v>7000</v>
+        <v>5000</v>
       </c>
       <c r="M40" s="16">
         <v>24</v>

</xml_diff>